<commit_message>
fix LR1, LR3, LR4
</commit_message>
<xml_diff>
--- a/LR3/table_1_12.xlsx
+++ b/LR3/table_1_12.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>№ квартиры</t>
   </si>
@@ -141,21 +141,12 @@
     <t xml:space="preserve"> Куропаткин 16</t>
   </si>
   <si>
-    <t>Пени за 1 день</t>
-  </si>
-  <si>
     <t>Максимальный срок просрочки, дней</t>
   </si>
   <si>
     <t>Фамилия квартиросъёмщика</t>
   </si>
   <si>
-    <t>дата начала года</t>
-  </si>
-  <si>
-    <t>Тариф, руб.</t>
-  </si>
-  <si>
     <t>Штраф, руб.</t>
   </si>
   <si>
@@ -171,10 +162,16 @@
     <t>Площадь, кв.м.</t>
   </si>
   <si>
-    <t>Сумма, руб./кв.м.</t>
-  </si>
-  <si>
     <t>Cредняя площадь, кв.м.</t>
+  </si>
+  <si>
+    <t>Тариф, руб./кв.м.</t>
+  </si>
+  <si>
+    <t>Сумма, руб.</t>
+  </si>
+  <si>
+    <t>Пени за 1 день, руб.</t>
   </si>
 </sst>
 </file>
@@ -538,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -552,7 +549,7 @@
     <col min="6" max="6" width="21.5546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" style="3" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="14.109375" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9.109375" style="3"/>
@@ -562,25 +559,23 @@
       <c r="A1" s="2">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>1</v>
@@ -592,13 +587,13 @@
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2218,16 +2213,16 @@
     </row>
     <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C40" s="7">
-        <f>SUM(K3:K38)</f>
-        <v>21936.600000000002</v>
+        <f>_xlfn.FLOOR.MATH(SUM(K3:K38))</f>
+        <v>21936</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C41" s="2">
         <f>AVERAGE(C3:C38)</f>
@@ -2236,7 +2231,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" s="2">
         <f>MAX(H3:H38)</f>
@@ -2245,7 +2240,7 @@
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C43" s="2">
         <f>MAX(E3:E38)</f>

</xml_diff>